<commit_message>
update timelog tuần 3
</commit_message>
<xml_diff>
--- a/Private/Vương/4. Timelog/PM_TimeLog_Vương.xlsx
+++ b/Private/Vương/4. Timelog/PM_TimeLog_Vương.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\Capstone-Project\Private\Vương\4. Timelog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Capstone-Project\Private\Vương\4. Timelog\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="94">
   <si>
     <t>Work in period</t>
   </si>
@@ -306,6 +306,18 @@
   </si>
   <si>
     <t>Install qgis</t>
+  </si>
+  <si>
+    <t>Research GIS</t>
+  </si>
+  <si>
+    <t>Install react</t>
+  </si>
+  <si>
+    <t>research react</t>
+  </si>
+  <si>
+    <t>Document quality management</t>
   </si>
 </sst>
 </file>
@@ -1009,6 +1021,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1025,18 +1049,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4110,17 +4122,17 @@
       <c r="I1" s="26"/>
     </row>
     <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="71"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="75"/>
     </row>
     <row r="3" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="29" t="s">
@@ -4320,21 +4332,21 @@
       <c r="B11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="66">
+      <c r="C11" s="70">
         <f>SUM(F4:F10)</f>
         <v>24</v>
       </c>
-      <c r="D11" s="66"/>
-      <c r="E11" s="66"/>
-      <c r="F11" s="67"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="71"/>
       <c r="G11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="66">
+      <c r="H11" s="70">
         <f>SUM(G4:G10)</f>
         <v>24</v>
       </c>
-      <c r="I11" s="67"/>
+      <c r="I11" s="71"/>
     </row>
     <row r="12" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
@@ -4508,21 +4520,21 @@
       <c r="B19" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="66">
+      <c r="C19" s="70">
         <f>SUM(F12:F18)</f>
         <v>22</v>
       </c>
-      <c r="D19" s="66"/>
-      <c r="E19" s="66"/>
-      <c r="F19" s="67"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="70"/>
+      <c r="F19" s="71"/>
       <c r="G19" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H19" s="66">
+      <c r="H19" s="70">
         <f>SUM(G12:G18)</f>
         <v>34</v>
       </c>
-      <c r="I19" s="67"/>
+      <c r="I19" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4555,10 +4567,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4586,17 +4598,17 @@
       <c r="I1" s="26"/>
     </row>
     <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="71"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="75"/>
     </row>
     <row r="3" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="29" t="s">
@@ -4769,7 +4781,7 @@
         <v>18</v>
       </c>
       <c r="D9" s="12"/>
-      <c r="E9" s="72">
+      <c r="E9" s="66">
         <v>43757</v>
       </c>
       <c r="F9" s="9">
@@ -4788,7 +4800,7 @@
       <c r="B10" s="13"/>
       <c r="C10" s="11"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="72"/>
+      <c r="E10" s="66"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="18"/>
@@ -4801,21 +4813,21 @@
       <c r="B11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="66">
+      <c r="C11" s="70">
         <f>SUM(F4:F10)</f>
         <v>26.5</v>
       </c>
-      <c r="D11" s="66"/>
-      <c r="E11" s="66"/>
-      <c r="F11" s="67"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="71"/>
       <c r="G11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="66">
+      <c r="H11" s="70">
         <f>SUM(G4:G10)</f>
         <v>27.5</v>
       </c>
-      <c r="I11" s="67"/>
+      <c r="I11" s="71"/>
     </row>
     <row r="12" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
@@ -4830,7 +4842,7 @@
       <c r="D12" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="E12" s="73">
+      <c r="E12" s="67">
         <v>43759</v>
       </c>
       <c r="F12" s="8">
@@ -4857,7 +4869,7 @@
       <c r="D13" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E13" s="74">
+      <c r="E13" s="68">
         <v>43760</v>
       </c>
       <c r="F13" s="8">
@@ -4882,7 +4894,7 @@
         <v>63</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="75">
+      <c r="E14" s="69">
         <v>43761</v>
       </c>
       <c r="F14" s="9">
@@ -4909,7 +4921,7 @@
       <c r="D15" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E15" s="74">
+      <c r="E15" s="68">
         <v>43762</v>
       </c>
       <c r="F15" s="9"/>
@@ -4932,7 +4944,7 @@
       <c r="D16" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E16" s="72">
+      <c r="E16" s="66">
         <v>43763</v>
       </c>
       <c r="F16" s="9"/>
@@ -4987,24 +4999,247 @@
       <c r="B19" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="66">
+      <c r="C19" s="70">
         <f>SUM(F12:F18)</f>
         <v>18.5</v>
       </c>
-      <c r="D19" s="66"/>
-      <c r="E19" s="66"/>
-      <c r="F19" s="67"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="70"/>
+      <c r="F19" s="71"/>
       <c r="G19" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H19" s="66">
+      <c r="H19" s="70">
         <f>SUM(G12:G18)</f>
         <v>22</v>
       </c>
-      <c r="I19" s="67"/>
+      <c r="I19" s="71"/>
+    </row>
+    <row r="20" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="12">
+        <v>3</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E21" s="67">
+        <v>43766</v>
+      </c>
+      <c r="F21" s="8">
+        <v>5</v>
+      </c>
+      <c r="G21" s="8">
+        <v>5</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="I21" s="19"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="12">
+        <v>3</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="17"/>
+      <c r="E22" s="68">
+        <v>43767</v>
+      </c>
+      <c r="F22" s="8">
+        <v>4</v>
+      </c>
+      <c r="G22" s="8">
+        <v>4</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="I22" s="19"/>
+    </row>
+    <row r="23" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="12">
+        <v>3</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="69">
+        <v>43768</v>
+      </c>
+      <c r="F23" s="9">
+        <v>4.5</v>
+      </c>
+      <c r="G23" s="9">
+        <v>5</v>
+      </c>
+      <c r="H23" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="12">
+        <v>3</v>
+      </c>
+      <c r="B24" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" s="68">
+        <v>43769</v>
+      </c>
+      <c r="F24" s="9">
+        <v>5</v>
+      </c>
+      <c r="G24" s="9">
+        <v>5</v>
+      </c>
+      <c r="H24" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="12">
+        <v>3</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25" s="66">
+        <v>43739</v>
+      </c>
+      <c r="F25" s="9">
+        <v>6</v>
+      </c>
+      <c r="G25" s="9">
+        <v>5</v>
+      </c>
+      <c r="H25" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="12">
+        <v>3</v>
+      </c>
+      <c r="B26" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E26" s="66">
+        <v>43740</v>
+      </c>
+      <c r="F26" s="9">
+        <v>5.5</v>
+      </c>
+      <c r="G26" s="9">
+        <v>5</v>
+      </c>
+      <c r="H26" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="11"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="5"/>
+    </row>
+    <row r="28" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="70">
+        <f>SUM(F21:F27)</f>
+        <v>30</v>
+      </c>
+      <c r="D28" s="70"/>
+      <c r="E28" s="70"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" s="70">
+        <f>SUM(G21:G27)</f>
+        <v>29</v>
+      </c>
+      <c r="I28" s="71"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="H28:I28"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="C11:F11"/>
     <mergeCell ref="H11:I11"/>
@@ -5012,16 +5247,16 @@
     <mergeCell ref="H19:I19"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C18">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C18 C27">
       <formula1>"Project Management, Requirement, Architecture and Desgin, Implementation, Testing, Training, Meetting Customer, Meetting Mentor"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12:C17 C9:D9 C4:C8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12:C17 C9:D9 C4:C8 C21:C26">
       <formula1>"Project Management, Requirement, Architecture and Desgin, Implementation, Testing, Training, Meetting Customer, Meeting Mentor"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H10 H12:H18">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H10 H12:H18 H21:H27">
       <formula1>"Done,Inprogress "</formula1>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3 B20">
       <formula1>B4</formula1>
       <formula2>B10</formula2>
     </dataValidation>
@@ -5036,7 +5271,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="A1:XFD1048576"/>
+      <selection activeCell="H11" sqref="A2:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5063,17 +5298,17 @@
       <c r="I1" s="26"/>
     </row>
     <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="71"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="75"/>
     </row>
     <row r="3" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="29" t="s">
@@ -5112,14 +5347,20 @@
         <v>9</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+        <v>18</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="67">
+        <v>43766</v>
+      </c>
+      <c r="F4" s="8">
+        <v>5</v>
+      </c>
+      <c r="G4" s="8">
+        <v>5</v>
+      </c>
       <c r="H4" s="18" t="s">
         <v>20</v>
       </c>
@@ -5133,14 +5374,18 @@
         <v>10</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="D5" s="17"/>
-      <c r="E5" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
+      <c r="E5" s="68">
+        <v>43767</v>
+      </c>
+      <c r="F5" s="8">
+        <v>4</v>
+      </c>
+      <c r="G5" s="8">
+        <v>4</v>
+      </c>
       <c r="H5" s="18" t="s">
         <v>20</v>
       </c>
@@ -5154,14 +5399,18 @@
         <v>11</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
+      <c r="E6" s="69">
+        <v>43768</v>
+      </c>
+      <c r="F6" s="9">
+        <v>4.5</v>
+      </c>
+      <c r="G6" s="9">
+        <v>5</v>
+      </c>
       <c r="H6" s="18" t="s">
         <v>20</v>
       </c>
@@ -5175,14 +5424,20 @@
         <v>12</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
+        <v>18</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" s="68">
+        <v>43769</v>
+      </c>
+      <c r="F7" s="9">
+        <v>5</v>
+      </c>
+      <c r="G7" s="9">
+        <v>5</v>
+      </c>
       <c r="H7" s="18" t="s">
         <v>20</v>
       </c>
@@ -5196,14 +5451,20 @@
         <v>13</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
+        <v>18</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E8" s="66">
+        <v>43739</v>
+      </c>
+      <c r="F8" s="9">
+        <v>6</v>
+      </c>
+      <c r="G8" s="9">
+        <v>5</v>
+      </c>
       <c r="H8" s="18" t="s">
         <v>20</v>
       </c>
@@ -5216,11 +5477,21 @@
       <c r="B9" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
+      <c r="C9" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E9" s="66">
+        <v>43740</v>
+      </c>
+      <c r="F9" s="9">
+        <v>5.5</v>
+      </c>
+      <c r="G9" s="9">
+        <v>5</v>
+      </c>
       <c r="H9" s="18" t="s">
         <v>20</v>
       </c>
@@ -5244,21 +5515,21 @@
       <c r="B11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="66">
+      <c r="C11" s="70">
         <f>SUM(F4:F10)</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="66"/>
-      <c r="E11" s="66"/>
-      <c r="F11" s="67"/>
+        <v>30</v>
+      </c>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="71"/>
       <c r="G11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="66">
+      <c r="H11" s="70">
         <f>SUM(G4:G10)</f>
-        <v>0</v>
-      </c>
-      <c r="I11" s="67"/>
+        <v>29</v>
+      </c>
+      <c r="I11" s="71"/>
     </row>
     <row r="12" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
@@ -5402,21 +5673,21 @@
       <c r="B19" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="66">
+      <c r="C19" s="70">
         <f>SUM(F12:F18)</f>
         <v>0</v>
       </c>
-      <c r="D19" s="66"/>
-      <c r="E19" s="66"/>
-      <c r="F19" s="67"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="70"/>
+      <c r="F19" s="71"/>
       <c r="G19" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H19" s="66">
+      <c r="H19" s="70">
         <f>SUM(G12:G18)</f>
         <v>0</v>
       </c>
-      <c r="I19" s="67"/>
+      <c r="I19" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -5442,5 +5713,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>